<commit_message>
Version 7 final changes
</commit_message>
<xml_diff>
--- a/BOMs/SolarChargerV2.xlsx
+++ b/BOMs/SolarChargerV2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcmul\OneDrive\Documents\GitHub\SolarCharger\BOMs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{4AE2F5FD-8040-4168-A6A5-F564BDDE00C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{67041DAE-8F7D-4AAA-BB0F-A45A2122F504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="87" uniqueCount="78">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="87" uniqueCount="79">
   <si>
     <t>Id</t>
   </si>
@@ -164,9 +164,6 @@
     <t>Solar_Cell</t>
   </si>
   <si>
-    <t>https://www.amazon.com/Treedix-Polysilicon-Polycrystalline-Encapsulated-Waterproof/dp/B0834MQDT8/ref=sr_1_10?crid=ZON6KL1ZVZ52&amp;keywords=10W%2Bsolar%2Bpanel&amp;qid=1649971502&amp;sprefix=10w%2Bsolar%2Bpanel%2Caps%2C145&amp;sr=8-10&amp;th=1</t>
-  </si>
-  <si>
     <t>Price</t>
   </si>
   <si>
@@ -267,6 +264,12 @@
   </si>
   <si>
     <t>cart</t>
+  </si>
+  <si>
+    <t>amazon.com/dp/B00OZC19AY/ref=emc_bcc_2_i?th=1</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/short/1jf4t9wm</t>
   </si>
 </sst>
 </file>
@@ -1132,10 +1135,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1161,7 +1164,7 @@
         <v>11</v>
       </c>
       <c r="F1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G1" t="s">
         <v>1</v>
@@ -1187,7 +1190,7 @@
         <v>1.81</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -1198,19 +1201,19 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F3" s="3">
         <v>0.74</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -1221,7 +1224,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1233,7 +1236,7 @@
         <v>0.45</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -1244,7 +1247,7 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1256,7 +1259,7 @@
         <v>0.1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -1267,7 +1270,7 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1279,7 +1282,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -1290,7 +1293,7 @@
         <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1302,7 +1305,7 @@
         <v>0.1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -1313,19 +1316,19 @@
         <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F8" s="3">
         <v>0.15</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -1336,7 +1339,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1348,7 +1351,7 @@
         <v>0.19</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -1371,7 +1374,7 @@
         <v>1.66</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -1382,19 +1385,19 @@
         <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F11" s="3">
         <v>0.54</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -1417,7 +1420,7 @@
         <v>2.95</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -1434,13 +1437,13 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F13" s="3">
         <v>1.01</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -1451,7 +1454,7 @@
         <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1463,7 +1466,7 @@
         <v>0.1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -1474,7 +1477,7 @@
         <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1486,7 +1489,7 @@
         <v>1.63</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -1497,7 +1500,7 @@
         <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1509,7 +1512,7 @@
         <v>0.1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
@@ -1520,7 +1523,7 @@
         <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1532,7 +1535,7 @@
         <v>0.1</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
@@ -1543,7 +1546,7 @@
         <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -1555,7 +1558,7 @@
         <v>0.1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -1566,7 +1569,7 @@
         <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -1578,7 +1581,7 @@
         <v>0.49</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
@@ -1589,7 +1592,7 @@
         <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1601,7 +1604,7 @@
         <v>0.2</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
@@ -1624,33 +1627,27 @@
         <v>17.989999999999998</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F23" s="3">
         <f>SUM(F2:F21)</f>
         <v>30.549999999999997</v>
       </c>
       <c r="G23" t="s">
-        <v>77</v>
-      </c>
-      <c r="H23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24">
-        <f>FDIST(2.6295,10,60)</f>
-        <v>1.005741712842814E-2</v>
+        <v>76</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G21" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G21" r:id="rId1" display="https://www.amazon.com/Treedix-Polysilicon-Polycrystalline-Encapsulated-Waterproof/dp/B0834MQDT8/ref=sr_1_10?crid=ZON6KL1ZVZ52&amp;keywords=10W%2Bsolar%2Bpanel&amp;qid=1649971502&amp;sprefix=10w%2Bsolar%2Bpanel%2Caps%2C145&amp;sr=8-10&amp;th=1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="G12" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="G2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="G17" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
@@ -1670,6 +1667,7 @@
     <hyperlink ref="G10" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
     <hyperlink ref="G7" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
     <hyperlink ref="G3" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="H23" r:id="rId21" xr:uid="{A43324FC-A43A-495C-891E-D300313E955A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>